<commit_message>
Add Procfile and update requirements.txt
</commit_message>
<xml_diff>
--- a/JaundiceTH.xlsx
+++ b/JaundiceTH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotempaz/Documents/Projects/SigiTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC256CC-258D-8A49-8BE7-0430A19406EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F7B641-5E20-1B42-8DD9-32AD24C70F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15500" activeTab="1" xr2:uid="{39BC5DFD-454C-5E46-8EBC-5B106C44167B}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15500" xr2:uid="{39BC5DFD-454C-5E46-8EBC-5B106C44167B}"/>
   </bookViews>
   <sheets>
     <sheet name="Photo38" sheetId="1" r:id="rId1"/>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97BF60FC-00D5-3E45-B2FF-DD79610CA565}">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,7 +455,7 @@
         <v>5.3230769230769228</v>
       </c>
       <c r="C3" s="1">
-        <v>7.338461538461539</v>
+        <v>7.3384615384615399</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2249,7 +2249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AE69C4-5297-994D-9CC1-654E70B578F9}">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>